<commit_message>
testing cz version of table
</commit_message>
<xml_diff>
--- a/src/main/resources/datasets/preference-table-example-cz.xlsx
+++ b/src/main/resources/datasets/preference-table-example-cz.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="14">
   <si>
-    <t xml:space="preserve">Doc</t>
+    <t xml:space="preserve">Prófa</t>
   </si>
   <si>
     <t xml:space="preserve">NE</t>
@@ -34,22 +34,22 @@
     <t xml:space="preserve">PREFERUJI</t>
   </si>
   <si>
-    <t xml:space="preserve">Grumpy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Happy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sleepy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bashful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sneezy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dopey</t>
+    <t xml:space="preserve">Rejpal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Štístko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dřímal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stydlín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kejchal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Šmudla</t>
   </si>
   <si>
     <t xml:space="preserve">vysvětlivky:</t>
@@ -234,10 +234,10 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>